<commit_message>
Agregando 0_reset_time.py Control del tiempo correcto Modificandole mejoritas a main y corrigiendo y agregando elementos visuales.
</commit_message>
<xml_diff>
--- a/docs/Niveles Lvls.xlsx
+++ b/docs/Niveles Lvls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\@ Projects Games Software Design\mk2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE07F0D-6290-42EA-AA58-6B50CD742384}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72B788D-DEBE-4EBD-83CA-7B334AD45171}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="1530" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="255" yWindow="1530" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -1092,7 +1092,7 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -12783,7 +12783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33054183-88CC-4C42-A605-AD18B09E7A88}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>